<commit_message>
added clock face intialization
</commit_message>
<xml_diff>
--- a/Lab3/define_tables.xlsx
+++ b/Lab3/define_tables.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -122,6 +122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +406,7 @@
   <dimension ref="A1:R63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:H62"/>
+      <selection activeCell="M29" sqref="M29:N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1135,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1189,8 +1190,23 @@
       <c r="H18" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="6"/>
+      <c r="K18">
+        <v>45</v>
+      </c>
+      <c r="L18" s="1">
+        <v>60</v>
+      </c>
+      <c r="M18" s="4">
+        <f>$K$18*COS(RADIANS($L18))+$J$3</f>
+        <v>86.5</v>
+      </c>
+      <c r="N18" s="4">
+        <f>$J$4-$K$18*SIN(RADIANS($L18))-4</f>
+        <v>7.0288568297002598</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>-6</v>
       </c>
@@ -1217,8 +1233,19 @@
       <c r="H19" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L19" s="1">
+        <v>30</v>
+      </c>
+      <c r="M19" s="4">
+        <f t="shared" ref="M19:M29" si="4">$K$18*COS(RADIANS($L19))+$J$3</f>
+        <v>102.97114317029974</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" ref="N19:N29" si="5">$J$4-$K$18*SIN(RADIANS($L19))-4</f>
+        <v>23.500000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>-12</v>
       </c>
@@ -1239,14 +1266,25 @@
         <v>7</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" ref="G20:G62" si="4">$J$4-$J$2*SIN(RADIANS($A20))</f>
+        <f t="shared" ref="G20:G62" si="6">$J$4-$J$2*SIN(RADIANS($A20))</f>
         <v>58.316467632710371</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
+        <f t="shared" si="4"/>
+        <v>109</v>
+      </c>
+      <c r="N20" s="4">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>-18</v>
       </c>
@@ -1267,14 +1305,25 @@
         <v>7</v>
       </c>
       <c r="G21" s="4">
+        <f t="shared" si="6"/>
+        <v>62.360679774997898</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="1">
+        <v>-30</v>
+      </c>
+      <c r="M21" s="4">
         <f t="shared" si="4"/>
-        <v>62.360679774997898</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102.97114317029974</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="5"/>
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>-24</v>
       </c>
@@ -1295,14 +1344,25 @@
         <v>7</v>
       </c>
       <c r="G22" s="4">
+        <f t="shared" si="6"/>
+        <v>66.269465723032013</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="1">
+        <v>-60</v>
+      </c>
+      <c r="M22" s="4">
         <f t="shared" si="4"/>
-        <v>66.269465723032013</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>86.5</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" si="5"/>
+        <v>84.97114317029974</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>-30</v>
       </c>
@@ -1323,14 +1383,25 @@
         <v>7</v>
       </c>
       <c r="G23" s="4">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="1">
+        <v>-90</v>
+      </c>
+      <c r="M23" s="4">
         <f t="shared" si="4"/>
-        <v>70</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="N23" s="4">
+        <f t="shared" si="5"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>-36</v>
       </c>
@@ -1351,14 +1422,25 @@
         <v>7</v>
       </c>
       <c r="G24" s="4">
+        <f t="shared" si="6"/>
+        <v>73.511410091698934</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="1">
+        <v>-120</v>
+      </c>
+      <c r="M24" s="4">
         <f t="shared" si="4"/>
-        <v>73.511410091698934</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41.500000000000014</v>
+      </c>
+      <c r="N24" s="4">
+        <f t="shared" si="5"/>
+        <v>84.97114317029974</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>-42</v>
       </c>
@@ -1379,14 +1461,25 @@
         <v>7</v>
       </c>
       <c r="G25" s="4">
+        <f t="shared" si="6"/>
+        <v>76.765224254354337</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="1">
+        <v>-150</v>
+      </c>
+      <c r="M25" s="4">
         <f t="shared" si="4"/>
-        <v>76.765224254354337</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25.02885682970026</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" si="5"/>
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>-48</v>
       </c>
@@ -1407,14 +1500,25 @@
         <v>7</v>
       </c>
       <c r="G26" s="4">
+        <f t="shared" si="6"/>
+        <v>79.725793019095761</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="1">
+        <v>-180</v>
+      </c>
+      <c r="M26" s="4">
         <f t="shared" si="4"/>
-        <v>79.725793019095761</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="N26" s="4">
+        <f t="shared" si="5"/>
+        <v>46.000000000000007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>-54</v>
       </c>
@@ -1435,14 +1539,25 @@
         <v>7</v>
       </c>
       <c r="G27" s="4">
+        <f t="shared" si="6"/>
+        <v>82.360679774997891</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="1">
+        <v>-210</v>
+      </c>
+      <c r="M27" s="4">
         <f t="shared" si="4"/>
-        <v>82.360679774997891</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25.02885682970026</v>
+      </c>
+      <c r="N27" s="4">
+        <f t="shared" si="5"/>
+        <v>23.499999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>-60</v>
       </c>
@@ -1463,14 +1578,25 @@
         <v>7</v>
       </c>
       <c r="G28" s="4">
+        <f t="shared" si="6"/>
+        <v>84.641016151377542</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="1">
+        <v>-240</v>
+      </c>
+      <c r="M28" s="4">
         <f t="shared" si="4"/>
-        <v>84.641016151377542</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41.499999999999979</v>
+      </c>
+      <c r="N28" s="4">
+        <f t="shared" si="5"/>
+        <v>7.028856829700274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>-66</v>
       </c>
@@ -1491,14 +1617,25 @@
         <v>7</v>
       </c>
       <c r="G29" s="4">
+        <f t="shared" si="6"/>
+        <v>86.541818305704027</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="1">
+        <v>-270</v>
+      </c>
+      <c r="M29" s="4">
         <f t="shared" si="4"/>
-        <v>86.541818305704027</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63.999999999999993</v>
+      </c>
+      <c r="N29" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>-72</v>
       </c>
@@ -1519,14 +1656,14 @@
         <v>7</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>88.042260651806146</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>-78</v>
       </c>
@@ -1547,14 +1684,14 @@
         <v>7</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>89.125904029352228</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>-84</v>
       </c>
@@ -1575,7 +1712,7 @@
         <v>7</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>89.780875814730933</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -1603,7 +1740,7 @@
         <v>7</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -1631,7 +1768,7 @@
         <v>7</v>
       </c>
       <c r="G34" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>89.780875814730933</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -1652,14 +1789,14 @@
         <v>12</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" ref="E35:E62" si="5">$J$2*COS(RADIANS($A35))+$J$3</f>
+        <f t="shared" ref="E35:E62" si="7">$J$2*COS(RADIANS($A35))+$J$3</f>
         <v>55.683532367289629</v>
       </c>
       <c r="F35" t="s">
         <v>7</v>
       </c>
       <c r="G35" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>89.125904029352228</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -1680,14 +1817,14 @@
         <v>12</v>
       </c>
       <c r="E36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>51.639320225002109</v>
       </c>
       <c r="F36" t="s">
         <v>7</v>
       </c>
       <c r="G36" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>88.042260651806146</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -1708,14 +1845,14 @@
         <v>12</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>47.730534276967987</v>
       </c>
       <c r="F37" t="s">
         <v>7</v>
       </c>
       <c r="G37" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>86.541818305704027</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -1736,14 +1873,14 @@
         <v>12</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44.000000000000007</v>
       </c>
       <c r="F38" t="s">
         <v>7</v>
       </c>
       <c r="G38" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>84.641016151377556</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -1764,14 +1901,14 @@
         <v>12</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>40.48858990830108</v>
       </c>
       <c r="F39" t="s">
         <v>7</v>
       </c>
       <c r="G39" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>82.360679774997891</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -1792,14 +1929,14 @@
         <v>12</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>37.23477574564567</v>
       </c>
       <c r="F40" t="s">
         <v>7</v>
       </c>
       <c r="G40" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>79.725793019095761</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -1820,14 +1957,14 @@
         <v>12</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>34.274206980904239</v>
       </c>
       <c r="F41" t="s">
         <v>7</v>
       </c>
       <c r="G41" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>76.765224254354337</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -1848,14 +1985,14 @@
         <v>12</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>31.639320225002109</v>
       </c>
       <c r="F42" t="s">
         <v>7</v>
       </c>
       <c r="G42" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>73.511410091698934</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -1876,14 +2013,14 @@
         <v>12</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>29.358983848622451</v>
       </c>
       <c r="F43" t="s">
         <v>7</v>
       </c>
       <c r="G43" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="H43" s="1" t="s">
@@ -1904,14 +2041,14 @@
         <v>12</v>
       </c>
       <c r="E44" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>27.458181694295973</v>
       </c>
       <c r="F44" t="s">
         <v>7</v>
       </c>
       <c r="G44" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>66.269465723032013</v>
       </c>
       <c r="H44" s="1" t="s">
@@ -1932,14 +2069,14 @@
         <v>12</v>
       </c>
       <c r="E45" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>25.957739348193861</v>
       </c>
       <c r="F45" t="s">
         <v>7</v>
       </c>
       <c r="G45" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>62.360679774997898</v>
       </c>
       <c r="H45" s="1" t="s">
@@ -1960,14 +2097,14 @@
         <v>12</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>24.874095970647772</v>
       </c>
       <c r="F46" t="s">
         <v>7</v>
       </c>
       <c r="G46" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>58.316467632710371</v>
       </c>
       <c r="H46" s="1" t="s">
@@ -1988,14 +2125,14 @@
         <v>12</v>
       </c>
       <c r="E47" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>24.219124185269067</v>
       </c>
       <c r="F47" t="s">
         <v>7</v>
       </c>
       <c r="G47" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>54.18113853070615</v>
       </c>
       <c r="H47" s="1" t="s">
@@ -2016,14 +2153,14 @@
         <v>12</v>
       </c>
       <c r="E48" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="F48" t="s">
         <v>7</v>
       </c>
       <c r="G48" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>50.000000000000007</v>
       </c>
       <c r="H48" s="1" t="s">
@@ -2044,14 +2181,14 @@
         <v>12</v>
       </c>
       <c r="E49" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>24.219124185269067</v>
       </c>
       <c r="F49" t="s">
         <v>7</v>
       </c>
       <c r="G49" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45.818861469293857</v>
       </c>
       <c r="H49" s="1" t="s">
@@ -2072,14 +2209,14 @@
         <v>12</v>
       </c>
       <c r="E50" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>24.87409597064778</v>
       </c>
       <c r="F50" t="s">
         <v>7</v>
       </c>
       <c r="G50" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>41.683532367289615</v>
       </c>
       <c r="H50" s="1" t="s">
@@ -2100,14 +2237,14 @@
         <v>12</v>
       </c>
       <c r="E51" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>25.957739348193854</v>
       </c>
       <c r="F51" t="s">
         <v>7</v>
       </c>
       <c r="G51" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37.639320225002109</v>
       </c>
       <c r="H51" s="1" t="s">
@@ -2128,14 +2265,14 @@
         <v>12</v>
       </c>
       <c r="E52" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>27.458181694295966</v>
       </c>
       <c r="F52" t="s">
         <v>7</v>
       </c>
       <c r="G52" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>33.730534276967987</v>
       </c>
       <c r="H52" s="1" t="s">
@@ -2156,14 +2293,14 @@
         <v>12</v>
       </c>
       <c r="E53" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>29.358983848622458</v>
       </c>
       <c r="F53" t="s">
         <v>7</v>
       </c>
       <c r="G53" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>29.999999999999996</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -2184,14 +2321,14 @@
         <v>12</v>
       </c>
       <c r="E54" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>31.639320225002095</v>
       </c>
       <c r="F54" t="s">
         <v>7</v>
       </c>
       <c r="G54" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>26.48858990830108</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -2212,14 +2349,14 @@
         <v>12</v>
       </c>
       <c r="E55" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>34.274206980904232</v>
       </c>
       <c r="F55" t="s">
         <v>7</v>
       </c>
       <c r="G55" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>23.23477574564567</v>
       </c>
       <c r="H55" s="1" t="s">
@@ -2240,14 +2377,14 @@
         <v>12</v>
       </c>
       <c r="E56" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>37.234775745645678</v>
       </c>
       <c r="F56" t="s">
         <v>7</v>
       </c>
       <c r="G56" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.274206980904225</v>
       </c>
       <c r="H56" s="1" t="s">
@@ -2268,14 +2405,14 @@
         <v>12</v>
       </c>
       <c r="E57" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>40.488589908301066</v>
       </c>
       <c r="F57" t="s">
         <v>7</v>
       </c>
       <c r="G57" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.639320225002109</v>
       </c>
       <c r="H57" s="1" t="s">
@@ -2296,14 +2433,14 @@
         <v>12</v>
       </c>
       <c r="E58" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>43.999999999999986</v>
       </c>
       <c r="F58" t="s">
         <v>7</v>
       </c>
       <c r="G58" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>15.358983848622465</v>
       </c>
       <c r="H58" s="1" t="s">
@@ -2324,14 +2461,14 @@
         <v>12</v>
       </c>
       <c r="E59" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>47.730534276968001</v>
       </c>
       <c r="F59" t="s">
         <v>7</v>
       </c>
       <c r="G59" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>13.458181694295959</v>
       </c>
       <c r="H59" s="1" t="s">
@@ -2352,14 +2489,14 @@
         <v>12</v>
       </c>
       <c r="E60" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>51.639320225002095</v>
       </c>
       <c r="F60" t="s">
         <v>7</v>
       </c>
       <c r="G60" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.957739348193861</v>
       </c>
       <c r="H60" s="1" t="s">
@@ -2380,14 +2517,14 @@
         <v>12</v>
       </c>
       <c r="E61" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>55.683532367289608</v>
       </c>
       <c r="F61" t="s">
         <v>7</v>
       </c>
       <c r="G61" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.87409597064778</v>
       </c>
       <c r="H61" s="1" t="s">
@@ -2408,14 +2545,14 @@
         <v>12</v>
       </c>
       <c r="E62" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>59.818861469293864</v>
       </c>
       <c r="F62" t="s">
         <v>7</v>
       </c>
       <c r="G62" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.219124185269067</v>
       </c>
       <c r="H62" s="1" t="s">

</xml_diff>